<commit_message>
update blank.xlsx because the previous one has a custom column width
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/blank.xlsx
+++ b/src/main/webapp/WEB-INF/books/blank.xlsx
@@ -1,73 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/zssessentials/src/main/webapp/WEB-INF/books/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE69F47B-FFD5-8847-829F-96A8B5F16582}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17620"/>
+    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{3ED75874-DEE8-0C4A-A28C-5AFA38A1FEAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color indexed="8"/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -79,21 +55,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -116,7 +91,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -128,7 +103,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -145,9 +120,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -175,14 +150,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -210,6 +202,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -361,18 +370,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E5E4CA0-1B74-9E41-B4A9-9DFFB634997D}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="2" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <pageMargins left="0.69791666666666663" right="0.69791666666666663" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>